<commit_message>
updated facility test data file
</commit_message>
<xml_diff>
--- a/testData/Classification_Facility.xlsx
+++ b/testData/Classification_Facility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VENKATESHAMKASANAGOT\Documents\MyWorkspace\EADMProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F44C7D0-974F-40ED-98CB-3496D5B14C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB3393A-E606-4944-9A29-340DBB7FA592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1781,15 +1781,6 @@
     <t>A grouping of assets that work together to dispose of the wastewater effluent product. (i.e. Evaporation / Infiltration ponds / etc)</t>
   </si>
   <si>
-    <t>A grouping of assets that work together to perform the function controlling a part of the business product provision,  i.e. a site pressure reduction facility within a network.</t>
-  </si>
-  <si>
-    <t>A grouping of assets that work together to perform the function pressure control for a part of the business product provision within a scheme,  i.e. a site pressure reduction facility within a network.</t>
-  </si>
-  <si>
-    <t>A grouping of assets that work together to perform the function pressure control for a part of the non-potable business product provision within a scheme,  i.e. a site pressure reduction facility within a network.</t>
-  </si>
-  <si>
     <t xml:space="preserve">A grouping of assets that work together to perform the function monitoring a part of the business product provision, i.e. a site monitoring the flow in the network away from any other facility. </t>
   </si>
   <si>
@@ -1873,6 +1864,15 @@
   </si>
   <si>
     <t>A collection of assets that provide reserve and emergency storage for (treated) potable water before it is distributed to customer to ensure not interrupted water supply (i.e.. due to a leak on the main) and ensure consistent water pressure. Type of tanks: Ground Level Tank or Elevated Tank.</t>
+  </si>
+  <si>
+    <t>A grouping of assets that work together to perform the function controlling a part of the business product provision, i.e. a site pressure reduction facility within a network.</t>
+  </si>
+  <si>
+    <t>A grouping of assets that work together to perform the function pressure control for a part of the business product provision within a scheme, i.e. a site pressure reduction facility within a network.</t>
+  </si>
+  <si>
+    <t>A grouping of assets that work together to perform the function pressure control for a part of the non-potable business product provision within a scheme, i.e. a site pressure reduction facility within a network.</t>
   </si>
 </sst>
 </file>
@@ -2840,8 +2840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3727,7 +3727,7 @@
         <v>346</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>574</v>
+        <v>596</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>13</v>
@@ -3895,7 +3895,7 @@
         <v>352</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>575</v>
+        <v>597</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>13</v>
@@ -3923,7 +3923,7 @@
         <v>353</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>576</v>
+        <v>598</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>13</v>
@@ -4179,7 +4179,7 @@
         <v>362</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>13</v>
@@ -4459,7 +4459,7 @@
         <v>372</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F57" s="17">
         <v>6120</v>
@@ -4575,7 +4575,7 @@
         <v>376</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F61" s="23">
         <v>6140</v>
@@ -4889,7 +4889,7 @@
         <v>387</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F72" s="17">
         <v>6330</v>
@@ -4919,7 +4919,7 @@
         <v>388</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F73" s="17">
         <v>6340</v>
@@ -4949,7 +4949,7 @@
         <v>389</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F74" s="17">
         <v>6350</v>
@@ -5005,7 +5005,7 @@
         <v>391</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F76" s="17">
         <v>6320</v>
@@ -5353,7 +5353,7 @@
         <v>403</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F88" s="23">
         <v>3140</v>
@@ -5527,7 +5527,7 @@
         <v>409</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F94" s="18" t="s">
         <v>13</v>
@@ -5843,7 +5843,7 @@
         <v>420</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F105" s="17">
         <v>2110</v>
@@ -5901,7 +5901,7 @@
         <v>422</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F107" s="18" t="s">
         <v>13</v>
@@ -5929,7 +5929,7 @@
         <v>423</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F108" s="17">
         <v>2210</v>
@@ -5959,7 +5959,7 @@
         <v>424</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F109" s="17">
         <v>2220</v>
@@ -5989,7 +5989,7 @@
         <v>425</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F110" s="17">
         <v>2230</v>
@@ -6019,7 +6019,7 @@
         <v>426</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F111" s="18" t="s">
         <v>13</v>
@@ -6077,7 +6077,7 @@
         <v>428</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F113" s="17">
         <v>2240</v>
@@ -6311,7 +6311,7 @@
         <v>436</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F121" s="18" t="s">
         <v>13</v>
@@ -6339,7 +6339,7 @@
         <v>437</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F122" s="18" t="s">
         <v>13</v>
@@ -6397,7 +6397,7 @@
         <v>439</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="F124" s="17">
         <v>2420</v>
@@ -6427,7 +6427,7 @@
         <v>440</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F125" s="17">
         <v>2430</v>
@@ -6457,7 +6457,7 @@
         <v>441</v>
       </c>
       <c r="E126" s="13" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F126" s="18" t="s">
         <v>13</v>
@@ -6485,7 +6485,7 @@
         <v>442</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F127" s="17">
         <v>2440</v>

</xml_diff>